<commit_message>
Finalização das alterações do projeto
</commit_message>
<xml_diff>
--- a/assets/planilhas/Dashboard-Tecnologia.xlsx
+++ b/assets/planilhas/Dashboard-Tecnologia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delab\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delab\OneDrive\Área de Trabalho\Planilhas-Excel\assets\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20541F9A-367D-4DB5-B9C6-17ABA5AAA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D818DA-564F-4631-A754-FD4F1A40D851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4618CA2-EC50-4E86-988A-DB3D773B87C6}"/>
+    <workbookView xWindow="996" yWindow="-108" windowWidth="22152" windowHeight="13176" activeTab="1" xr2:uid="{C4618CA2-EC50-4E86-988A-DB3D773B87C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
@@ -770,9 +770,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF7C3F58"/>
       <color rgb="FFEB6B6F"/>
       <color rgb="FFFFF6D3"/>
-      <color rgb="FF7C3F58"/>
       <color rgb="FFF9A875"/>
     </mruColors>
   </colors>
@@ -1063,7 +1063,7 @@
                   <c:v>16431.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3974.9700000000003</c:v>
+                  <c:v>4058.0700000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1609,7 +1609,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2950.4400000000005</c:v>
+                  <c:v>3033.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4343.87</c:v>
@@ -3862,15 +3862,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>215320</xdr:colOff>
+      <xdr:colOff>168667</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>3258</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>235434</xdr:colOff>
+      <xdr:colOff>264367</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>10878</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="$I$4">
       <xdr:nvSpPr>
@@ -3885,8 +3885,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4504516" y="180680"/>
-          <a:ext cx="1858341" cy="730342"/>
+          <a:off x="4414096" y="189870"/>
+          <a:ext cx="1915169" cy="754069"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3928,7 +3928,7 @@
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t> R$ 68,938.17 </a:t>
+            <a:t> R$ 69,021.27 </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -3967,13 +3967,13 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>183693</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>3346</xdr:rowOff>
+      <xdr:rowOff>3332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>220546</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>10817</xdr:rowOff>
+      <xdr:rowOff>10803</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="$N$4">
       <xdr:nvSpPr>
@@ -3988,8 +3988,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6889293" y="183455"/>
-          <a:ext cx="1865653" cy="727907"/>
+          <a:off x="6855081" y="189944"/>
+          <a:ext cx="1856322" cy="753920"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -4138,13 +4138,13 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>168805</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>6515</xdr:rowOff>
+      <xdr:rowOff>3258</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>472033</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>31102</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>14135</xdr:rowOff>
+      <xdr:rowOff>10878</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="$R$3">
       <xdr:nvSpPr>
@@ -4159,8 +4159,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9312805" y="190291"/>
-          <a:ext cx="2741628" cy="742726"/>
+          <a:off x="9266152" y="189870"/>
+          <a:ext cx="2894746" cy="754069"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -4194,7 +4194,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:fld id="{5062E6E1-40D5-4CC1-9BAC-4F84A68524C0}" type="TxLink">
-            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="7C3F58"/>
               </a:solidFill>
@@ -4204,7 +4204,7 @@
             <a:pPr algn="ctr"/>
             <a:t>Galaxy S23 Ultra</a:t>
           </a:fld>
-          <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:srgbClr val="7C3F58"/>
             </a:solidFill>
@@ -4222,7 +4222,7 @@
               <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Produto Mais Vendido</a:t>
+            <a:t>Produto de Maior Faturamento</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4392,13 +4392,173 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>326571</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101081</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>93307</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38878</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Agrupar 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480AD98C-DE92-3E32-882A-7F3C5F420B58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11849877" y="101081"/>
+          <a:ext cx="979716" cy="311021"/>
+          <a:chOff x="11849877" y="101081"/>
+          <a:chExt cx="979716" cy="311021"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="$Q$3">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Retângulo: Cantos Arredondados 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE3EC519-7659-4A50-13DA-8B765BDBDF20}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11849877" y="101081"/>
+            <a:ext cx="979716" cy="311021"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="EB6B6F"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="7C3F58"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="r"/>
+            <a:fld id="{7CB66636-4940-4916-853D-8B99EF83CBE6}" type="TxLink">
+              <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="7C3F58"/>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:pPr algn="r"/>
+              <a:t>21725.7</a:t>
+            </a:fld>
+            <a:endParaRPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="7C3F58"/>
+              </a:solidFill>
+              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="CaixaDeTexto 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A475DC3-7D68-F5F5-54DE-982434109D99}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11849877" y="110800"/>
+            <a:ext cx="396551" cy="291583"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1000" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="7C3F58"/>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>R$</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4436,7 +4596,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4542,7 +4702,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4684,7 +4844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4694,8 +4854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59995A85-B102-42F9-9E3F-F59EF24784C6}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5057,7 +5217,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="1">
-        <v>59.8</v>
+        <v>87.5</v>
       </c>
       <c r="F11" s="22" t="s">
         <v>27</v>
@@ -5079,7 +5239,7 @@
       </c>
       <c r="L11" s="44">
         <f t="shared" si="0"/>
-        <v>179.39999999999998</v>
+        <v>262.5</v>
       </c>
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
@@ -5689,8 +5849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520B442F-79B5-4E16-A449-B7070042AF89}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5720,7 +5880,7 @@
       </c>
       <c r="I4" s="49">
         <f>SUM(Produtos!L4:L26)</f>
-        <v>68938.17</v>
+        <v>69021.27</v>
       </c>
       <c r="J4" s="49"/>
       <c r="M4" s="7" t="s">
@@ -5754,7 +5914,7 @@
       </c>
       <c r="D10" s="10">
         <f>SUMIFS(Produtos!L4:L26, Produtos!G4:G26, Gráficos!C10)</f>
-        <v>2950.4400000000005</v>
+        <v>3033.54</v>
       </c>
       <c r="E10" s="8"/>
       <c r="O10" s="8"/>
@@ -5823,7 +5983,7 @@
       </c>
       <c r="Q13" s="14">
         <f>SUMIFS(Produtos!L4:L26, Produtos!H4:H26, Gráficos!P13)</f>
-        <v>3974.9700000000003</v>
+        <v>4058.0700000000006</v>
       </c>
       <c r="R13" s="8"/>
     </row>

</xml_diff>

<commit_message>
Adição do segundo projeto
Dashboard para organização de catálogo de livros
</commit_message>
<xml_diff>
--- a/assets/planilhas/Dashboard-Tecnologia.xlsx
+++ b/assets/planilhas/Dashboard-Tecnologia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delab\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delab\OneDrive\Área de Trabalho\Planilhas-Excel\assets\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20541F9A-367D-4DB5-B9C6-17ABA5AAA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D818DA-564F-4631-A754-FD4F1A40D851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4618CA2-EC50-4E86-988A-DB3D773B87C6}"/>
+    <workbookView xWindow="996" yWindow="-108" windowWidth="22152" windowHeight="13176" activeTab="1" xr2:uid="{C4618CA2-EC50-4E86-988A-DB3D773B87C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
@@ -770,9 +770,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF7C3F58"/>
       <color rgb="FFEB6B6F"/>
       <color rgb="FFFFF6D3"/>
-      <color rgb="FF7C3F58"/>
       <color rgb="FFF9A875"/>
     </mruColors>
   </colors>
@@ -1063,7 +1063,7 @@
                   <c:v>16431.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3974.9700000000003</c:v>
+                  <c:v>4058.0700000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1609,7 +1609,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2950.4400000000005</c:v>
+                  <c:v>3033.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4343.87</c:v>
@@ -3862,15 +3862,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>215320</xdr:colOff>
+      <xdr:colOff>168667</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>3258</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>235434</xdr:colOff>
+      <xdr:colOff>264367</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>10878</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="$I$4">
       <xdr:nvSpPr>
@@ -3885,8 +3885,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4504516" y="180680"/>
-          <a:ext cx="1858341" cy="730342"/>
+          <a:off x="4414096" y="189870"/>
+          <a:ext cx="1915169" cy="754069"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3928,7 +3928,7 @@
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t> R$ 68,938.17 </a:t>
+            <a:t> R$ 69,021.27 </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -3967,13 +3967,13 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>183693</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>3346</xdr:rowOff>
+      <xdr:rowOff>3332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>220546</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>10817</xdr:rowOff>
+      <xdr:rowOff>10803</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="$N$4">
       <xdr:nvSpPr>
@@ -3988,8 +3988,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6889293" y="183455"/>
-          <a:ext cx="1865653" cy="727907"/>
+          <a:off x="6855081" y="189944"/>
+          <a:ext cx="1856322" cy="753920"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -4138,13 +4138,13 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>168805</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>6515</xdr:rowOff>
+      <xdr:rowOff>3258</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>472033</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>31102</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>14135</xdr:rowOff>
+      <xdr:rowOff>10878</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="$R$3">
       <xdr:nvSpPr>
@@ -4159,8 +4159,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9312805" y="190291"/>
-          <a:ext cx="2741628" cy="742726"/>
+          <a:off x="9266152" y="189870"/>
+          <a:ext cx="2894746" cy="754069"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -4194,7 +4194,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:fld id="{5062E6E1-40D5-4CC1-9BAC-4F84A68524C0}" type="TxLink">
-            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="7C3F58"/>
               </a:solidFill>
@@ -4204,7 +4204,7 @@
             <a:pPr algn="ctr"/>
             <a:t>Galaxy S23 Ultra</a:t>
           </a:fld>
-          <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:srgbClr val="7C3F58"/>
             </a:solidFill>
@@ -4222,7 +4222,7 @@
               <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Produto Mais Vendido</a:t>
+            <a:t>Produto de Maior Faturamento</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4392,13 +4392,173 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>326571</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101081</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>93307</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38878</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Agrupar 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480AD98C-DE92-3E32-882A-7F3C5F420B58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11849877" y="101081"/>
+          <a:ext cx="979716" cy="311021"/>
+          <a:chOff x="11849877" y="101081"/>
+          <a:chExt cx="979716" cy="311021"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="$Q$3">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Retângulo: Cantos Arredondados 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE3EC519-7659-4A50-13DA-8B765BDBDF20}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11849877" y="101081"/>
+            <a:ext cx="979716" cy="311021"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="EB6B6F"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="7C3F58"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="r"/>
+            <a:fld id="{7CB66636-4940-4916-853D-8B99EF83CBE6}" type="TxLink">
+              <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="7C3F58"/>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:pPr algn="r"/>
+              <a:t>21725.7</a:t>
+            </a:fld>
+            <a:endParaRPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="7C3F58"/>
+              </a:solidFill>
+              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="CaixaDeTexto 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A475DC3-7D68-F5F5-54DE-982434109D99}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11849877" y="110800"/>
+            <a:ext cx="396551" cy="291583"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1000" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="7C3F58"/>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>R$</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4436,7 +4596,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4542,7 +4702,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4684,7 +4844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4694,8 +4854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59995A85-B102-42F9-9E3F-F59EF24784C6}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5057,7 +5217,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="1">
-        <v>59.8</v>
+        <v>87.5</v>
       </c>
       <c r="F11" s="22" t="s">
         <v>27</v>
@@ -5079,7 +5239,7 @@
       </c>
       <c r="L11" s="44">
         <f t="shared" si="0"/>
-        <v>179.39999999999998</v>
+        <v>262.5</v>
       </c>
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
@@ -5689,8 +5849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520B442F-79B5-4E16-A449-B7070042AF89}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5720,7 +5880,7 @@
       </c>
       <c r="I4" s="49">
         <f>SUM(Produtos!L4:L26)</f>
-        <v>68938.17</v>
+        <v>69021.27</v>
       </c>
       <c r="J4" s="49"/>
       <c r="M4" s="7" t="s">
@@ -5754,7 +5914,7 @@
       </c>
       <c r="D10" s="10">
         <f>SUMIFS(Produtos!L4:L26, Produtos!G4:G26, Gráficos!C10)</f>
-        <v>2950.4400000000005</v>
+        <v>3033.54</v>
       </c>
       <c r="E10" s="8"/>
       <c r="O10" s="8"/>
@@ -5823,7 +5983,7 @@
       </c>
       <c r="Q13" s="14">
         <f>SUMIFS(Produtos!L4:L26, Produtos!H4:H26, Gráficos!P13)</f>
-        <v>3974.9700000000003</v>
+        <v>4058.0700000000006</v>
       </c>
       <c r="R13" s="8"/>
     </row>

</xml_diff>